<commit_message>
back to original function
</commit_message>
<xml_diff>
--- a/code/PSNR.xlsx
+++ b/code/PSNR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\github\Digital_Watermarking-LSB-pair\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ABD28683-836D-473C-A9E0-7BA333230410}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{63FEF467-F9AB-4C5F-AEF3-759EC1EF072B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20865" windowHeight="10590" xr2:uid="{ECC0FC8B-ECD6-49CB-AAEE-DFAD19D18CF4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20865" windowHeight="10590" xr2:uid="{047A2B34-79FB-436B-9C99-017AA34A6AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Image Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,15 +35,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LSB-DES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSB-pair</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSB-pair1</t>
+    <t>LSB-pair-ultar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,16 +467,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA438ACE-CA1F-428B-9733-83ABB97AD5DB}">
-  <dimension ref="A1:E101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3EDE64-3313-4595-BCB7-E58CABA61B58}">
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E101"/>
+      <selection activeCell="B2" sqref="B2:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,13 +487,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -509,16 +498,13 @@
         <v>44545</v>
       </c>
       <c r="C2">
-        <v>43922</v>
+        <v>44554</v>
       </c>
       <c r="D2">
-        <v>43922</v>
-      </c>
-      <c r="E2">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -526,16 +512,13 @@
         <v>43913</v>
       </c>
       <c r="C3">
-        <v>43991</v>
+        <v>43921</v>
       </c>
       <c r="D3">
-        <v>43991</v>
-      </c>
-      <c r="E3">
-        <v>43991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>100</v>
       </c>
@@ -543,16 +526,13 @@
         <v>44591</v>
       </c>
       <c r="C4">
-        <v>43833</v>
+        <v>44599</v>
       </c>
       <c r="D4">
-        <v>43833</v>
-      </c>
-      <c r="E4">
-        <v>43833</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44591</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -560,16 +540,13 @@
         <v>44696</v>
       </c>
       <c r="C5">
-        <v>44038</v>
+        <v>44710</v>
       </c>
       <c r="D5">
-        <v>44038</v>
-      </c>
-      <c r="E5">
-        <v>44038</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -577,16 +554,13 @@
         <v>44008</v>
       </c>
       <c r="C6">
-        <v>44074</v>
+        <v>44016</v>
       </c>
       <c r="D6">
-        <v>44074</v>
-      </c>
-      <c r="E6">
-        <v>44074</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13</v>
       </c>
@@ -594,16 +568,13 @@
         <v>43010</v>
       </c>
       <c r="C7">
-        <v>43689</v>
+        <v>43010</v>
       </c>
       <c r="D7">
-        <v>43689</v>
-      </c>
-      <c r="E7">
-        <v>43689</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>43010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14</v>
       </c>
@@ -611,16 +582,13 @@
         <v>37346</v>
       </c>
       <c r="C8">
-        <v>43848</v>
+        <v>37354</v>
       </c>
       <c r="D8">
-        <v>43848</v>
-      </c>
-      <c r="E8">
-        <v>43848</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>15</v>
       </c>
@@ -628,16 +596,13 @@
         <v>43421</v>
       </c>
       <c r="C9">
-        <v>44176</v>
+        <v>43426</v>
       </c>
       <c r="D9">
-        <v>44176</v>
-      </c>
-      <c r="E9">
-        <v>44176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>43421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16</v>
       </c>
@@ -645,16 +610,13 @@
         <v>43274</v>
       </c>
       <c r="C10">
-        <v>43758</v>
+        <v>43283</v>
       </c>
       <c r="D10">
-        <v>43758</v>
-      </c>
-      <c r="E10">
-        <v>43758</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>43274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>17</v>
       </c>
@@ -662,16 +624,13 @@
         <v>45613</v>
       </c>
       <c r="C11">
-        <v>43959</v>
+        <v>45620</v>
       </c>
       <c r="D11">
-        <v>43959</v>
-      </c>
-      <c r="E11">
-        <v>43959</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>0</v>
       </c>
@@ -681,11 +640,8 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>0</v>
       </c>
@@ -695,11 +651,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>0</v>
       </c>
@@ -709,11 +662,8 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>0</v>
       </c>
@@ -723,11 +673,8 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>0</v>
       </c>
@@ -737,11 +684,8 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>0</v>
       </c>
@@ -751,11 +695,8 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>0</v>
       </c>
@@ -765,11 +706,8 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>0</v>
       </c>
@@ -779,11 +717,8 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>0</v>
       </c>
@@ -793,11 +728,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>0</v>
       </c>
@@ -807,11 +739,8 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>0</v>
       </c>
@@ -821,11 +750,8 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>0</v>
       </c>
@@ -835,11 +761,8 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>0</v>
       </c>
@@ -849,11 +772,8 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>0</v>
       </c>
@@ -863,11 +783,8 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>0</v>
       </c>
@@ -877,11 +794,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>0</v>
       </c>
@@ -891,11 +805,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>0</v>
       </c>
@@ -905,11 +816,8 @@
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>0</v>
       </c>
@@ -919,11 +827,8 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>0</v>
       </c>
@@ -933,11 +838,8 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>0</v>
       </c>
@@ -947,11 +849,8 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>0</v>
       </c>
@@ -961,11 +860,8 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33">
         <v>0</v>
       </c>
@@ -975,11 +871,8 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34">
         <v>0</v>
       </c>
@@ -989,11 +882,8 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35">
         <v>0</v>
       </c>
@@ -1003,11 +893,8 @@
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1017,11 +904,8 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37">
         <v>0</v>
       </c>
@@ -1031,11 +915,8 @@
       <c r="D37">
         <v>0</v>
       </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38">
         <v>0</v>
       </c>
@@ -1045,11 +926,8 @@
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39">
         <v>0</v>
       </c>
@@ -1059,11 +937,8 @@
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40">
         <v>0</v>
       </c>
@@ -1073,11 +948,8 @@
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41">
         <v>0</v>
       </c>
@@ -1087,11 +959,8 @@
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42">
         <v>0</v>
       </c>
@@ -1101,11 +970,8 @@
       <c r="D42">
         <v>0</v>
       </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>0</v>
       </c>
@@ -1115,11 +981,8 @@
       <c r="D43">
         <v>0</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>0</v>
       </c>
@@ -1129,11 +992,8 @@
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>0</v>
       </c>
@@ -1143,11 +1003,8 @@
       <c r="D45">
         <v>0</v>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46">
         <v>0</v>
       </c>
@@ -1157,11 +1014,8 @@
       <c r="D46">
         <v>0</v>
       </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>0</v>
       </c>
@@ -1171,11 +1025,8 @@
       <c r="D47">
         <v>0</v>
       </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48">
         <v>0</v>
       </c>
@@ -1185,11 +1036,8 @@
       <c r="D48">
         <v>0</v>
       </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>0</v>
       </c>
@@ -1199,11 +1047,8 @@
       <c r="D49">
         <v>0</v>
       </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>0</v>
       </c>
@@ -1213,11 +1058,8 @@
       <c r="D50">
         <v>0</v>
       </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>0</v>
       </c>
@@ -1227,11 +1069,8 @@
       <c r="D51">
         <v>0</v>
       </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52">
         <v>0</v>
       </c>
@@ -1241,11 +1080,8 @@
       <c r="D52">
         <v>0</v>
       </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53">
         <v>0</v>
       </c>
@@ -1255,11 +1091,8 @@
       <c r="D53">
         <v>0</v>
       </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>0</v>
       </c>
@@ -1269,11 +1102,8 @@
       <c r="D54">
         <v>0</v>
       </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>0</v>
       </c>
@@ -1283,11 +1113,8 @@
       <c r="D55">
         <v>0</v>
       </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>0</v>
       </c>
@@ -1297,11 +1124,8 @@
       <c r="D56">
         <v>0</v>
       </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>0</v>
       </c>
@@ -1311,11 +1135,8 @@
       <c r="D57">
         <v>0</v>
       </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58">
         <v>0</v>
       </c>
@@ -1325,11 +1146,8 @@
       <c r="D58">
         <v>0</v>
       </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59">
         <v>0</v>
       </c>
@@ -1339,11 +1157,8 @@
       <c r="D59">
         <v>0</v>
       </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60">
         <v>0</v>
       </c>
@@ -1353,11 +1168,8 @@
       <c r="D60">
         <v>0</v>
       </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61">
         <v>0</v>
       </c>
@@ -1367,11 +1179,8 @@
       <c r="D61">
         <v>0</v>
       </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62">
         <v>0</v>
       </c>
@@ -1381,11 +1190,8 @@
       <c r="D62">
         <v>0</v>
       </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>0</v>
       </c>
@@ -1395,11 +1201,8 @@
       <c r="D63">
         <v>0</v>
       </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>0</v>
       </c>
@@ -1409,11 +1212,8 @@
       <c r="D64">
         <v>0</v>
       </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65">
         <v>0</v>
       </c>
@@ -1423,11 +1223,8 @@
       <c r="D65">
         <v>0</v>
       </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66">
         <v>0</v>
       </c>
@@ -1437,11 +1234,8 @@
       <c r="D66">
         <v>0</v>
       </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67">
         <v>0</v>
       </c>
@@ -1451,11 +1245,8 @@
       <c r="D67">
         <v>0</v>
       </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68">
         <v>0</v>
       </c>
@@ -1465,11 +1256,8 @@
       <c r="D68">
         <v>0</v>
       </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69">
         <v>0</v>
       </c>
@@ -1479,11 +1267,8 @@
       <c r="D69">
         <v>0</v>
       </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70">
         <v>0</v>
       </c>
@@ -1493,11 +1278,8 @@
       <c r="D70">
         <v>0</v>
       </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71">
         <v>0</v>
       </c>
@@ -1507,11 +1289,8 @@
       <c r="D71">
         <v>0</v>
       </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72">
         <v>0</v>
       </c>
@@ -1521,11 +1300,8 @@
       <c r="D72">
         <v>0</v>
       </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73">
         <v>0</v>
       </c>
@@ -1535,11 +1311,8 @@
       <c r="D73">
         <v>0</v>
       </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74">
         <v>0</v>
       </c>
@@ -1549,11 +1322,8 @@
       <c r="D74">
         <v>0</v>
       </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75">
         <v>0</v>
       </c>
@@ -1563,11 +1333,8 @@
       <c r="D75">
         <v>0</v>
       </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>0</v>
       </c>
@@ -1577,11 +1344,8 @@
       <c r="D76">
         <v>0</v>
       </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>0</v>
       </c>
@@ -1591,11 +1355,8 @@
       <c r="D77">
         <v>0</v>
       </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78">
         <v>0</v>
       </c>
@@ -1605,11 +1366,8 @@
       <c r="D78">
         <v>0</v>
       </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>0</v>
       </c>
@@ -1619,11 +1377,8 @@
       <c r="D79">
         <v>0</v>
       </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80">
         <v>0</v>
       </c>
@@ -1633,11 +1388,8 @@
       <c r="D80">
         <v>0</v>
       </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81">
         <v>0</v>
       </c>
@@ -1647,11 +1399,8 @@
       <c r="D81">
         <v>0</v>
       </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>0</v>
       </c>
@@ -1661,11 +1410,8 @@
       <c r="D82">
         <v>0</v>
       </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>0</v>
       </c>
@@ -1675,11 +1421,8 @@
       <c r="D83">
         <v>0</v>
       </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84">
         <v>0</v>
       </c>
@@ -1689,11 +1432,8 @@
       <c r="D84">
         <v>0</v>
       </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85">
         <v>0</v>
       </c>
@@ -1703,11 +1443,8 @@
       <c r="D85">
         <v>0</v>
       </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>0</v>
       </c>
@@ -1717,11 +1454,8 @@
       <c r="D86">
         <v>0</v>
       </c>
-      <c r="E86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>0</v>
       </c>
@@ -1731,11 +1465,8 @@
       <c r="D87">
         <v>0</v>
       </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88">
         <v>0</v>
       </c>
@@ -1745,11 +1476,8 @@
       <c r="D88">
         <v>0</v>
       </c>
-      <c r="E88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>0</v>
       </c>
@@ -1759,11 +1487,8 @@
       <c r="D89">
         <v>0</v>
       </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90">
         <v>0</v>
       </c>
@@ -1773,11 +1498,8 @@
       <c r="D90">
         <v>0</v>
       </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91">
         <v>0</v>
       </c>
@@ -1787,11 +1509,8 @@
       <c r="D91">
         <v>0</v>
       </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92">
         <v>0</v>
       </c>
@@ -1801,11 +1520,8 @@
       <c r="D92">
         <v>0</v>
       </c>
-      <c r="E92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93">
         <v>0</v>
       </c>
@@ -1815,11 +1531,8 @@
       <c r="D93">
         <v>0</v>
       </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94">
         <v>0</v>
       </c>
@@ -1829,11 +1542,8 @@
       <c r="D94">
         <v>0</v>
       </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95">
         <v>0</v>
       </c>
@@ -1843,11 +1553,8 @@
       <c r="D95">
         <v>0</v>
       </c>
-      <c r="E95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96">
         <v>0</v>
       </c>
@@ -1857,11 +1564,8 @@
       <c r="D96">
         <v>0</v>
       </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97">
         <v>0</v>
       </c>
@@ -1871,11 +1575,8 @@
       <c r="D97">
         <v>0</v>
       </c>
-      <c r="E97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98">
         <v>0</v>
       </c>
@@ -1885,11 +1586,8 @@
       <c r="D98">
         <v>0</v>
       </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99">
         <v>0</v>
       </c>
@@ -1899,11 +1597,8 @@
       <c r="D99">
         <v>0</v>
       </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100">
         <v>0</v>
       </c>
@@ -1913,11 +1608,8 @@
       <c r="D100">
         <v>0</v>
       </c>
-      <c r="E100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101">
         <v>0</v>
       </c>
@@ -1925,9 +1617,6 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <v>0</v>
-      </c>
-      <c r="E101">
         <v>0</v>
       </c>
     </row>

</xml_diff>